<commit_message>
processed a bunch of msa continuum files
</commit_message>
<xml_diff>
--- a/raw_data/local_continuum/Cleveland.xlsx
+++ b/raw_data/local_continuum/Cleveland.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10614"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melissaschnure/Dropbox/Documents_local/Hopkins/PhD/EHE/Suppression data/31. Cleveland/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Todd Fojo\CloudStation\Projects\Ending HIV\Ending_HIV\raw_data\local_continuum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7860084C-EDF3-2348-987E-1C35172ADA80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="18120" windowHeight="19440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="18120" windowHeight="19440" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Stratified_Data" sheetId="6" r:id="rId1"/>
@@ -18,7 +17,7 @@
     <sheet name="Comments" sheetId="2" r:id="rId3"/>
     <sheet name="Indicator definitions" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,17 +35,26 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>tc={51D9DE27-C023-D543-ACE0-E2D96F4536B3}</author>
   </authors>
   <commentList>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{51D9DE27-C023-D543-ACE0-E2D96F4536B3}">
+    <comment ref="C1" authorId="0" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     3 months</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -54,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="72">
   <si>
     <t>Total</t>
   </si>
@@ -271,12 +279,15 @@
   </si>
   <si>
     <t>Region 3/Part A-Cleveland data</t>
+  </si>
+  <si>
+    <t>https://odh.ohio.gov/wps/wcm/connect/gov/c36c5c0e-f795-476b-9ebe-4d39946406fa/Region+3+HIV+Care+Continuum+2018.pdf?MOD=AJPERES&amp;CONVERT_TO=url&amp;CACHEID=ROOTWORKSPACE.Z18_M1HGGIK0N0JO00QO9DDDDM3000-c36c5c0e-f795-476b-9ebe-4d39946406fa-niOebGY</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -836,22 +847,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E718E012-04A8-3E48-894F-E2D70020E78C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AX33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:49" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -1000,7 +1011,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:49" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:49" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -1149,7 +1160,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="3" spans="1:49" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:49" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -1330,7 +1341,7 @@
         <v>0.27675421403371225</v>
       </c>
     </row>
-    <row r="4" spans="1:49" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:49" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
@@ -1447,7 +1458,7 @@
       <c r="AV4" s="40"/>
       <c r="AW4" s="41"/>
     </row>
-    <row r="5" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -1564,7 +1575,7 @@
       <c r="AV5" s="46"/>
       <c r="AW5" s="47"/>
     </row>
-    <row r="6" spans="1:49" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:49" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -1681,7 +1692,7 @@
       <c r="AV6" s="52"/>
       <c r="AW6" s="53"/>
     </row>
-    <row r="7" spans="1:49" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:49" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>4</v>
       </c>
@@ -1798,7 +1809,7 @@
       <c r="AV7" s="40"/>
       <c r="AW7" s="41"/>
     </row>
-    <row r="8" spans="1:49" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:49" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
@@ -1915,7 +1926,7 @@
       <c r="AV8" s="52"/>
       <c r="AW8" s="53"/>
     </row>
-    <row r="9" spans="1:49" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:49" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>6</v>
       </c>
@@ -2040,7 +2051,7 @@
       <c r="AV9" s="40"/>
       <c r="AW9" s="39"/>
     </row>
-    <row r="10" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -2165,7 +2176,7 @@
       <c r="AV10" s="46"/>
       <c r="AW10" s="47"/>
     </row>
-    <row r="11" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -2290,7 +2301,7 @@
       <c r="AV11" s="46"/>
       <c r="AW11" s="45"/>
     </row>
-    <row r="12" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -2415,7 +2426,7 @@
       <c r="AV12" s="46"/>
       <c r="AW12" s="47"/>
     </row>
-    <row r="13" spans="1:49" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:49" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
@@ -2540,7 +2551,7 @@
       <c r="AV13" s="46"/>
       <c r="AW13" s="51"/>
     </row>
-    <row r="14" spans="1:49" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:49" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>11</v>
       </c>
@@ -2656,7 +2667,7 @@
       <c r="AV14" s="41"/>
       <c r="AW14" s="41"/>
     </row>
-    <row r="15" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
@@ -2780,7 +2791,7 @@
       <c r="AV15" s="46"/>
       <c r="AW15" s="47"/>
     </row>
-    <row r="16" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
@@ -2896,7 +2907,7 @@
       <c r="AV16" s="46"/>
       <c r="AW16" s="47"/>
     </row>
-    <row r="17" spans="1:50" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:50" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>14</v>
       </c>
@@ -3020,7 +3031,7 @@
       <c r="AV17" s="53"/>
       <c r="AW17" s="53"/>
     </row>
-    <row r="18" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>20</v>
       </c>
@@ -3090,7 +3101,7 @@
       <c r="AW18" s="47"/>
       <c r="AX18" s="14"/>
     </row>
-    <row r="19" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:50" x14ac:dyDescent="0.3">
       <c r="H19" s="12"/>
       <c r="I19" s="13"/>
       <c r="J19" s="12"/>
@@ -3112,7 +3123,7 @@
       <c r="AC19" s="13"/>
       <c r="AE19" s="12"/>
     </row>
-    <row r="20" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:50" x14ac:dyDescent="0.3">
       <c r="B20" s="47" t="s">
         <v>69</v>
       </c>
@@ -3131,7 +3142,7 @@
       <c r="Y20" s="12"/>
       <c r="AE20" s="12"/>
     </row>
-    <row r="21" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:50" x14ac:dyDescent="0.3">
       <c r="B21" s="50" t="s">
         <v>45</v>
       </c>
@@ -3140,49 +3151,49 @@
       <c r="Y21" s="15"/>
       <c r="AE21" s="15"/>
     </row>
-    <row r="22" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:50" x14ac:dyDescent="0.3">
       <c r="M22" s="12"/>
       <c r="S22" s="12"/>
       <c r="Y22" s="12"/>
       <c r="AE22" s="12"/>
     </row>
-    <row r="23" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:50" x14ac:dyDescent="0.3">
       <c r="M23" s="15"/>
       <c r="S23" s="15"/>
       <c r="Y23" s="15"/>
       <c r="AE23" s="15"/>
     </row>
-    <row r="24" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:50" x14ac:dyDescent="0.3">
       <c r="M24" s="15"/>
       <c r="S24" s="15"/>
       <c r="Y24" s="15"/>
       <c r="AE24" s="15"/>
     </row>
-    <row r="26" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:50" x14ac:dyDescent="0.3">
       <c r="M26" s="12"/>
       <c r="S26" s="12"/>
       <c r="Y26" s="12"/>
       <c r="AE26" s="12"/>
     </row>
-    <row r="27" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:50" x14ac:dyDescent="0.3">
       <c r="M27" s="12"/>
       <c r="S27" s="12"/>
       <c r="Y27" s="12"/>
       <c r="AE27" s="12"/>
     </row>
-    <row r="28" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:50" x14ac:dyDescent="0.3">
       <c r="M28" s="12"/>
       <c r="S28" s="12"/>
       <c r="Y28" s="12"/>
       <c r="AE28" s="12"/>
     </row>
-    <row r="29" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:50" x14ac:dyDescent="0.3">
       <c r="M29" s="12"/>
       <c r="S29" s="12"/>
       <c r="Y29" s="12"/>
       <c r="AE29" s="12"/>
     </row>
-    <row r="30" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:50" x14ac:dyDescent="0.3">
       <c r="F30" t="s">
         <v>23</v>
       </c>
@@ -3191,19 +3202,19 @@
       <c r="Y30" s="12"/>
       <c r="AE30" s="12"/>
     </row>
-    <row r="31" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:50" x14ac:dyDescent="0.3">
       <c r="M31" s="12"/>
       <c r="S31" s="12"/>
       <c r="Y31" s="12"/>
       <c r="AE31" s="12"/>
     </row>
-    <row r="32" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:50" x14ac:dyDescent="0.3">
       <c r="M32" s="12"/>
       <c r="S32" s="12"/>
       <c r="Y32" s="12"/>
       <c r="AE32" s="12"/>
     </row>
-    <row r="33" spans="13:31" x14ac:dyDescent="0.2">
+    <row r="33" spans="13:31" x14ac:dyDescent="0.3">
       <c r="M33" s="12"/>
       <c r="S33" s="12"/>
       <c r="Y33" s="12"/>
@@ -3216,7 +3227,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F596BA49-69CC-F54C-A2C6-F75D688FD882}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
@@ -3226,12 +3237,12 @@
       <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -3254,7 +3265,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>2015</v>
       </c>
@@ -3281,7 +3292,7 @@
         <v>0.27675421403371225</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2016</v>
       </c>
@@ -3308,7 +3319,7 @@
         <v>0.43360640121927985</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2017</v>
       </c>
@@ -3335,7 +3346,7 @@
         <v>0.58090136682674542</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>2018</v>
       </c>
@@ -3362,7 +3373,7 @@
         <v>0.62875226039783005</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>2015</v>
       </c>
@@ -3389,7 +3400,7 @@
         <v>0.43554549313711616</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>2016</v>
       </c>
@@ -3416,7 +3427,7 @@
         <v>0.4770324300310973</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>2017</v>
       </c>
@@ -3443,7 +3454,7 @@
         <v>0.53676883835545375</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>2018</v>
       </c>
@@ -3470,14 +3481,14 @@
         <v>0.59022524436889079</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B11" s="47" t="s">
         <v>70</v>
       </c>
       <c r="C11" s="47"/>
       <c r="D11" s="47"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B12" s="50" t="s">
         <v>45</v>
       </c>
@@ -3490,28 +3501,31 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="J2" s="9"/>
       <c r="K2" s="9"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>64</v>
       </c>
@@ -3519,15 +3533,15 @@
         <v>1235072</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B5" s="30"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>65</v>
       </c>
@@ -3535,7 +3549,7 @@
         <v>309833</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>66</v>
       </c>
@@ -3546,7 +3560,7 @@
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>67</v>
       </c>
@@ -3554,7 +3568,7 @@
         <v>179746</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>68</v>
       </c>
@@ -3562,134 +3576,134 @@
         <v>93649</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="10"/>
       <c r="B13" s="31"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="10"/>
       <c r="B14" s="31"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>46</v>
       </c>
       <c r="B15" s="16"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B24" s="57" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B27" s="57" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B29" s="8" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B30" s="8" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B31" s="8" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B32" s="8" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B33" s="8" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B39" s="8"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B29" r:id="rId1" xr:uid="{50F42068-6FF2-EE48-A267-E79BEA15EE76}"/>
-    <hyperlink ref="B31" r:id="rId2" xr:uid="{CAD72B80-5B4B-9249-AA0C-7D735921B14A}"/>
-    <hyperlink ref="B32" r:id="rId3" xr:uid="{F43FB697-67A2-AE4A-A107-5BA98083644F}"/>
-    <hyperlink ref="B30" r:id="rId4" xr:uid="{1CE42D07-63E6-A348-B106-78D0E5626E95}"/>
-    <hyperlink ref="B33" r:id="rId5" xr:uid="{19E71A97-F095-D649-9577-030D0E1F4DF0}"/>
+    <hyperlink ref="B29" r:id="rId1"/>
+    <hyperlink ref="B31" r:id="rId2"/>
+    <hyperlink ref="B32" r:id="rId3"/>
+    <hyperlink ref="B30" r:id="rId4"/>
+    <hyperlink ref="B33" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B9CD82F-C49B-E645-9ED1-742B79A009E4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="52" customWidth="1"/>
     <col min="3" max="3" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>28</v>
       </c>
@@ -3700,7 +3714,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
         <v>31</v>
       </c>
@@ -3709,7 +3723,7 @@
       </c>
       <c r="C2" s="23"/>
     </row>
-    <row r="3" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="24" t="s">
         <v>30</v>
       </c>
@@ -3720,7 +3734,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="26" t="s">
         <v>32</v>
       </c>
@@ -3729,7 +3743,7 @@
       </c>
       <c r="C4" s="23"/>
     </row>
-    <row r="5" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="26" t="s">
         <v>33</v>
       </c>
@@ -3740,7 +3754,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="26" t="s">
         <v>39</v>
       </c>
@@ -3751,7 +3765,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="26" t="s">
         <v>41</v>
       </c>
@@ -3762,69 +3776,69 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="29" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B9" s="16"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B10" s="16"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B11" s="16"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B12" s="16"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B13" s="16"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B14" s="16"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B15" s="16"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B16" s="16"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" s="16"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" s="16"/>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" s="16"/>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" s="16"/>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B21" s="16"/>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B22" s="16"/>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B23" s="16"/>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B24" s="16"/>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B25" s="16"/>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B26" s="16"/>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B27" s="16"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- processed a bunch of msa continuum files - fixed cache issue - updated ui   - new tabs   - spinner appears when loading plots (done/WIP)   - Fixed location widget selection issue
</commit_message>
<xml_diff>
--- a/raw_data/local_continuum/Cleveland.xlsx
+++ b/raw_data/local_continuum/Cleveland.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10614"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melissaschnure/Dropbox/Documents_local/Hopkins/PhD/EHE/Suppression data/31. Cleveland/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Todd Fojo\CloudStation\Projects\Ending HIV\Ending_HIV\raw_data\local_continuum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7860084C-EDF3-2348-987E-1C35172ADA80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="18120" windowHeight="19440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="18120" windowHeight="19440" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Stratified_Data" sheetId="6" r:id="rId1"/>
@@ -18,7 +17,7 @@
     <sheet name="Comments" sheetId="2" r:id="rId3"/>
     <sheet name="Indicator definitions" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,17 +35,26 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>tc={51D9DE27-C023-D543-ACE0-E2D96F4536B3}</author>
   </authors>
   <commentList>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{51D9DE27-C023-D543-ACE0-E2D96F4536B3}">
+    <comment ref="C1" authorId="0" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     3 months</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -54,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="72">
   <si>
     <t>Total</t>
   </si>
@@ -271,12 +279,15 @@
   </si>
   <si>
     <t>Region 3/Part A-Cleveland data</t>
+  </si>
+  <si>
+    <t>https://odh.ohio.gov/wps/wcm/connect/gov/c36c5c0e-f795-476b-9ebe-4d39946406fa/Region+3+HIV+Care+Continuum+2018.pdf?MOD=AJPERES&amp;CONVERT_TO=url&amp;CACHEID=ROOTWORKSPACE.Z18_M1HGGIK0N0JO00QO9DDDDM3000-c36c5c0e-f795-476b-9ebe-4d39946406fa-niOebGY</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -836,22 +847,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E718E012-04A8-3E48-894F-E2D70020E78C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AX33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:49" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -1000,7 +1011,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:49" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:49" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -1149,7 +1160,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="3" spans="1:49" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:49" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -1330,7 +1341,7 @@
         <v>0.27675421403371225</v>
       </c>
     </row>
-    <row r="4" spans="1:49" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:49" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
@@ -1447,7 +1458,7 @@
       <c r="AV4" s="40"/>
       <c r="AW4" s="41"/>
     </row>
-    <row r="5" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -1564,7 +1575,7 @@
       <c r="AV5" s="46"/>
       <c r="AW5" s="47"/>
     </row>
-    <row r="6" spans="1:49" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:49" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -1681,7 +1692,7 @@
       <c r="AV6" s="52"/>
       <c r="AW6" s="53"/>
     </row>
-    <row r="7" spans="1:49" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:49" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>4</v>
       </c>
@@ -1798,7 +1809,7 @@
       <c r="AV7" s="40"/>
       <c r="AW7" s="41"/>
     </row>
-    <row r="8" spans="1:49" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:49" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
@@ -1915,7 +1926,7 @@
       <c r="AV8" s="52"/>
       <c r="AW8" s="53"/>
     </row>
-    <row r="9" spans="1:49" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:49" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>6</v>
       </c>
@@ -2040,7 +2051,7 @@
       <c r="AV9" s="40"/>
       <c r="AW9" s="39"/>
     </row>
-    <row r="10" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -2165,7 +2176,7 @@
       <c r="AV10" s="46"/>
       <c r="AW10" s="47"/>
     </row>
-    <row r="11" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -2290,7 +2301,7 @@
       <c r="AV11" s="46"/>
       <c r="AW11" s="45"/>
     </row>
-    <row r="12" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -2415,7 +2426,7 @@
       <c r="AV12" s="46"/>
       <c r="AW12" s="47"/>
     </row>
-    <row r="13" spans="1:49" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:49" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
@@ -2540,7 +2551,7 @@
       <c r="AV13" s="46"/>
       <c r="AW13" s="51"/>
     </row>
-    <row r="14" spans="1:49" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:49" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>11</v>
       </c>
@@ -2656,7 +2667,7 @@
       <c r="AV14" s="41"/>
       <c r="AW14" s="41"/>
     </row>
-    <row r="15" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
@@ -2780,7 +2791,7 @@
       <c r="AV15" s="46"/>
       <c r="AW15" s="47"/>
     </row>
-    <row r="16" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
@@ -2896,7 +2907,7 @@
       <c r="AV16" s="46"/>
       <c r="AW16" s="47"/>
     </row>
-    <row r="17" spans="1:50" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:50" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>14</v>
       </c>
@@ -3020,7 +3031,7 @@
       <c r="AV17" s="53"/>
       <c r="AW17" s="53"/>
     </row>
-    <row r="18" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>20</v>
       </c>
@@ -3090,7 +3101,7 @@
       <c r="AW18" s="47"/>
       <c r="AX18" s="14"/>
     </row>
-    <row r="19" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:50" x14ac:dyDescent="0.3">
       <c r="H19" s="12"/>
       <c r="I19" s="13"/>
       <c r="J19" s="12"/>
@@ -3112,7 +3123,7 @@
       <c r="AC19" s="13"/>
       <c r="AE19" s="12"/>
     </row>
-    <row r="20" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:50" x14ac:dyDescent="0.3">
       <c r="B20" s="47" t="s">
         <v>69</v>
       </c>
@@ -3131,7 +3142,7 @@
       <c r="Y20" s="12"/>
       <c r="AE20" s="12"/>
     </row>
-    <row r="21" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:50" x14ac:dyDescent="0.3">
       <c r="B21" s="50" t="s">
         <v>45</v>
       </c>
@@ -3140,49 +3151,49 @@
       <c r="Y21" s="15"/>
       <c r="AE21" s="15"/>
     </row>
-    <row r="22" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:50" x14ac:dyDescent="0.3">
       <c r="M22" s="12"/>
       <c r="S22" s="12"/>
       <c r="Y22" s="12"/>
       <c r="AE22" s="12"/>
     </row>
-    <row r="23" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:50" x14ac:dyDescent="0.3">
       <c r="M23" s="15"/>
       <c r="S23" s="15"/>
       <c r="Y23" s="15"/>
       <c r="AE23" s="15"/>
     </row>
-    <row r="24" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:50" x14ac:dyDescent="0.3">
       <c r="M24" s="15"/>
       <c r="S24" s="15"/>
       <c r="Y24" s="15"/>
       <c r="AE24" s="15"/>
     </row>
-    <row r="26" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:50" x14ac:dyDescent="0.3">
       <c r="M26" s="12"/>
       <c r="S26" s="12"/>
       <c r="Y26" s="12"/>
       <c r="AE26" s="12"/>
     </row>
-    <row r="27" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:50" x14ac:dyDescent="0.3">
       <c r="M27" s="12"/>
       <c r="S27" s="12"/>
       <c r="Y27" s="12"/>
       <c r="AE27" s="12"/>
     </row>
-    <row r="28" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:50" x14ac:dyDescent="0.3">
       <c r="M28" s="12"/>
       <c r="S28" s="12"/>
       <c r="Y28" s="12"/>
       <c r="AE28" s="12"/>
     </row>
-    <row r="29" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:50" x14ac:dyDescent="0.3">
       <c r="M29" s="12"/>
       <c r="S29" s="12"/>
       <c r="Y29" s="12"/>
       <c r="AE29" s="12"/>
     </row>
-    <row r="30" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:50" x14ac:dyDescent="0.3">
       <c r="F30" t="s">
         <v>23</v>
       </c>
@@ -3191,19 +3202,19 @@
       <c r="Y30" s="12"/>
       <c r="AE30" s="12"/>
     </row>
-    <row r="31" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:50" x14ac:dyDescent="0.3">
       <c r="M31" s="12"/>
       <c r="S31" s="12"/>
       <c r="Y31" s="12"/>
       <c r="AE31" s="12"/>
     </row>
-    <row r="32" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:50" x14ac:dyDescent="0.3">
       <c r="M32" s="12"/>
       <c r="S32" s="12"/>
       <c r="Y32" s="12"/>
       <c r="AE32" s="12"/>
     </row>
-    <row r="33" spans="13:31" x14ac:dyDescent="0.2">
+    <row r="33" spans="13:31" x14ac:dyDescent="0.3">
       <c r="M33" s="12"/>
       <c r="S33" s="12"/>
       <c r="Y33" s="12"/>
@@ -3216,7 +3227,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F596BA49-69CC-F54C-A2C6-F75D688FD882}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
@@ -3226,12 +3237,12 @@
       <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -3254,7 +3265,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>2015</v>
       </c>
@@ -3281,7 +3292,7 @@
         <v>0.27675421403371225</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2016</v>
       </c>
@@ -3308,7 +3319,7 @@
         <v>0.43360640121927985</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2017</v>
       </c>
@@ -3335,7 +3346,7 @@
         <v>0.58090136682674542</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>2018</v>
       </c>
@@ -3362,7 +3373,7 @@
         <v>0.62875226039783005</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>2015</v>
       </c>
@@ -3389,7 +3400,7 @@
         <v>0.43554549313711616</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>2016</v>
       </c>
@@ -3416,7 +3427,7 @@
         <v>0.4770324300310973</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>2017</v>
       </c>
@@ -3443,7 +3454,7 @@
         <v>0.53676883835545375</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>2018</v>
       </c>
@@ -3470,14 +3481,14 @@
         <v>0.59022524436889079</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B11" s="47" t="s">
         <v>70</v>
       </c>
       <c r="C11" s="47"/>
       <c r="D11" s="47"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B12" s="50" t="s">
         <v>45</v>
       </c>
@@ -3490,28 +3501,31 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="J2" s="9"/>
       <c r="K2" s="9"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>64</v>
       </c>
@@ -3519,15 +3533,15 @@
         <v>1235072</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B5" s="30"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>65</v>
       </c>
@@ -3535,7 +3549,7 @@
         <v>309833</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>66</v>
       </c>
@@ -3546,7 +3560,7 @@
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>67</v>
       </c>
@@ -3554,7 +3568,7 @@
         <v>179746</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>68</v>
       </c>
@@ -3562,134 +3576,134 @@
         <v>93649</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="10"/>
       <c r="B13" s="31"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="10"/>
       <c r="B14" s="31"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>46</v>
       </c>
       <c r="B15" s="16"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B24" s="57" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B27" s="57" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B29" s="8" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B30" s="8" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B31" s="8" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B32" s="8" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B33" s="8" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B39" s="8"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B29" r:id="rId1" xr:uid="{50F42068-6FF2-EE48-A267-E79BEA15EE76}"/>
-    <hyperlink ref="B31" r:id="rId2" xr:uid="{CAD72B80-5B4B-9249-AA0C-7D735921B14A}"/>
-    <hyperlink ref="B32" r:id="rId3" xr:uid="{F43FB697-67A2-AE4A-A107-5BA98083644F}"/>
-    <hyperlink ref="B30" r:id="rId4" xr:uid="{1CE42D07-63E6-A348-B106-78D0E5626E95}"/>
-    <hyperlink ref="B33" r:id="rId5" xr:uid="{19E71A97-F095-D649-9577-030D0E1F4DF0}"/>
+    <hyperlink ref="B29" r:id="rId1"/>
+    <hyperlink ref="B31" r:id="rId2"/>
+    <hyperlink ref="B32" r:id="rId3"/>
+    <hyperlink ref="B30" r:id="rId4"/>
+    <hyperlink ref="B33" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B9CD82F-C49B-E645-9ED1-742B79A009E4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="52" customWidth="1"/>
     <col min="3" max="3" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>28</v>
       </c>
@@ -3700,7 +3714,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
         <v>31</v>
       </c>
@@ -3709,7 +3723,7 @@
       </c>
       <c r="C2" s="23"/>
     </row>
-    <row r="3" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="24" t="s">
         <v>30</v>
       </c>
@@ -3720,7 +3734,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="26" t="s">
         <v>32</v>
       </c>
@@ -3729,7 +3743,7 @@
       </c>
       <c r="C4" s="23"/>
     </row>
-    <row r="5" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="26" t="s">
         <v>33</v>
       </c>
@@ -3740,7 +3754,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="26" t="s">
         <v>39</v>
       </c>
@@ -3751,7 +3765,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="26" t="s">
         <v>41</v>
       </c>
@@ -3762,69 +3776,69 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="29" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B9" s="16"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B10" s="16"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B11" s="16"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B12" s="16"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B13" s="16"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B14" s="16"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B15" s="16"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B16" s="16"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" s="16"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" s="16"/>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" s="16"/>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" s="16"/>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B21" s="16"/>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B22" s="16"/>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B23" s="16"/>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B24" s="16"/>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B25" s="16"/>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B26" s="16"/>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B27" s="16"/>
     </row>
   </sheetData>

</xml_diff>